<commit_message>
Feat:" 씬 1~4 연결"
</commit_message>
<xml_diff>
--- a/hohoPlanet/Assets/Resources/ExcelDB/DialogueDB.xlsx
+++ b/hohoPlanet/Assets/Resources/ExcelDB/DialogueDB.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5ED82D-6BBE-4FCD-B6CB-3DB833F1C539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B43CF5-1898-4634-B32E-F5B3C3F3110F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="136">
   <si>
     <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,482 +65,495 @@
     <t>None</t>
   </si>
   <si>
-    <t>BackGround/00000</t>
+    <t>Character/00000</t>
+  </si>
+  <si>
+    <t>네! 그럼 다녀오겠습니다</t>
+  </si>
+  <si>
+    <t>소리가….더 커졌어!</t>
+  </si>
+  <si>
+    <t>근처에 얼마나 더 있는 거지?</t>
+  </si>
+  <si>
+    <t>to be continued</t>
+  </si>
+  <si>
+    <t>호호야 돌아왔느냐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앗 족장님!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠시 산책을 나갔다 왔어요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그랬구나…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>족장님? 무슨일 있으세요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혹시 마을 주변에서 이상한 것을 보지는 못했니?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이상한 것이요? 아뇨 보지 못했어요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">에휴… 그렇구나.. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 괜히 걱정하는 건가…</t>
+  </si>
+  <si>
+    <t>걱정하는게 있으세요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…그래 호호야 최근 인간이라고 하는 생명체들이 우리 행성에 온 것은 알고 있지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네 저희 행성이 아름답다고 잠시 머물면서 조사해도 되냐고 물었잖아요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리고 저희는 행성을 다치게 하지 않는 선에서 허락했구요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하지만 나는 요즘 인간들이 무척이나 의심스럽구나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인간들이 의심스럽다구요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래 최근 무언가 달라진 느낌을 많아 받는구나…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>숲속에 동물들이 많이 보이지 않고 무엇보다 이상한 소음이 늘었어…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호호야 내가 부탁하나 해도 되겠느냐?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">숲속을 순찰하면서 이상한 것들이 있는지 조사하고 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인간들이 숲속의 변화에 상관이 있는지 알아봐주렴…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 괜한 의심을 하는 걸지도 모르지만…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네 그럼요! 족장님의 부탁이신걸요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제가 뭘 도와드리면 될까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠시만 호호야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혹시 모르니 너에게 몸을 지킬 수 있는 방법을 알려주마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지킬 수 있는 방법이요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래 WASD를 이용하여 몸을 이동시키고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Space Bar를 눌러 여우 구슬을 발사하렴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리 행성의 부족들이 대대로 부족을 지키는 데 이용한 힘이란다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>으으 아파라…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>숲속에 왜 저런게 있지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혹시 모르니 주변을 좀 더 살펴봐야겠어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일단 마을로 돌아가서 족장님께 말씀드려야(쫑긋)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위이이잉 위이이잉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무슨 소리지? 뭐가 위이잉거렸는데?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>흠… 저 소리가 무엇인지만 확인하고 가야겠어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>족장님 의심대로 인간들이 한건가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여우 구슬로도 부술 수 없고... 다른 물건들과 다르게 아프진 않았지만 수상해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>확실히 무슨일이 벌어지고 있는 것 확실한것 같네...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일단 조심히 마을로 돌아가ㅇ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>으아 들켰다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헉헉헉 정말 힘들었어 그리고 저 물체들 점점 더 빨리져서 더 힘들었지…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래도 주변에 있는 것들은 다 처리 한 것 같으니까 이젠 정말 돌아가야겠어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위이이이이이이이잉!!!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위우우웅 위이이이이이잉!!!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삐빅 자원.. 수집 한다… 자우언으…ㅅ우이집…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>말소리?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>누군가 있나?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">말을 이상하게 하긴 하지만 누군가 다친 것 수도 있으니까 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도와주려 가야겠어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>왜 이렇게 위험한 것들이 많아진거지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리 호호족들만 있었을때는 이런일이 일어나지 않았어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그럼 정말 족장님의 의심대로 인간들이 벌인 짓인가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 행성 @$^%&amp;$ 수집#%@$%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>또 말소리가 들리잖아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그러게 원래도 좀 고장이 났어지만 이정도는 아니였는데…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어쨌든 이 행성의 자원에 대해서는 거의 다 조사했어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래? 결과는?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리 지구로 돌아가서도 충분이 사용이 가능한 자원들이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지구의 에너지 고갈 사태에 충분한 해결책이 될 것 같아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래 그럼 이 행성의 원주민들이 알아차리기 전에 최대한 많은 자원을 채굴하자고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하! 저 착해빠지고 멍청한 놈들은 우리의 허무맹랑한 소리도 믿었어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근데 만약 원주민들이 알게 되면 어떻게하지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래 그럼 곧 철수하지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방금 무슨 소리 못들었나?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소리? 뭐가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>흠… 아니다 잘못 들은 모양이군 가지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>말도 안돼… 우리 행성을 자원을 빼앗고 여차하면 공격하겠다니…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어서 이 사실을 족장님께 말씀드려야지!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주호마을</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인간들이 돌아가고 난 후</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>족장님!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호호야 돌아왔구나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이상한 물체들이 날라와 우리를 공격했단다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하지만 걱정 말거라 여우구슬의 힘으로 부족이 힘을 합쳐 물리쳤으니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">그래서 숲속에 이상한 것들을 만들었고 무엇보다 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리고 만약 알게 되더라도 우리가 가지고 있는 장비들을 사용해 모두 처리하면 그만이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래 알려줘서 고맙구나 호호야 수고했단다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래… 다른 부족장들과 상의해서 그들을 이 행성에 머물수 있도록 허락했지..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리고 위험할 수 있으니 인간을 마주친다면 숨으려무나…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네! 그럼 다녀오겠ㅅ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여우 구슬이요? 그게 뭐죠?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">이 힘으로 자신과, 부족을 지켜주렴 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네 족장님 인간… 마을이 왜 망가진거죠?!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다행이다… 아 맞다. 족장님 의심이 맞았어요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">인간들은 저의 행성을 연구하는 것이 아닌 자원을 훔치려 온거였어요 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">하긴 그렇긴 하지 그럼 이제 본부로 돌아가자 이 지역에 관한 정보는 거의 다 얻었어 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">이제 다른 지역으로 가도 될 것 같아 이곳을 마지막으로 이 행성의 지역별 자원에 대한 정보는 다 얻었어  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이제 본부로 돌아가서 본격적으로 자원을 채굴하자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로봇103-1177호가 망가졌군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호호야 위험하지만 인간들은 본부에 대해 조사를 해봐야겠구나..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일단 우리가 인간들에 대해 가진 정보가 너무 부족하니…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>만약 최악의 상황이 막치면 이 행성의 모든 부족들을 불러 모아 인간들과 전쟁을 할 수 도 있겠구나…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">일단 마을을 정비하자꾸나 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리고 준비 해야지 앞으로 우리 부족에게 닥칠 일을…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이번엔 몰래 접근 해야겠어…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">만약 저희가 자기들의 계획을 알게되면 저희를 다 처리할 거라고… </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리고 본부로 돌아간 다음 다른 지역으로 옮겨 본격적으로 자원을 채굴할 것이라고 했어요</t>
+  </si>
+  <si>
+    <t>네!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character/00001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주호 족장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">말까지 하는 이상한 물체.. 정말 위험했어. 대체 숲속에서 무슨일이 일어나고 있는거야 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>???</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인간1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인간2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바스락! (헉!)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map1</t>
+  </si>
+  <si>
+    <t>BackGround/00002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>BackGround/00001</t>
-  </si>
-  <si>
-    <t>Character/00000</t>
-  </si>
-  <si>
-    <t>네! 그럼 다녀오겠습니다</t>
-  </si>
-  <si>
-    <t>소리가….더 커졌어!</t>
-  </si>
-  <si>
-    <t>근처에 얼마나 더 있는 거지?</t>
-  </si>
-  <si>
-    <t>to be continued</t>
-  </si>
-  <si>
-    <t>호호야 돌아왔느냐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>앗 족장님!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잠시 산책을 나갔다 왔어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그랬구나…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>족장님? 무슨일 있으세요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>혹시 마을 주변에서 이상한 것을 보지는 못했니?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이상한 것이요? 아뇨 보지 못했어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">에휴… 그렇구나.. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내가 괜히 걱정하는 건가…</t>
-  </si>
-  <si>
-    <t>걱정하는게 있으세요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…그래 호호야 최근 인간이라고 하는 생명체들이 우리 행성에 온 것은 알고 있지?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네 저희 행성이 아름답다고 잠시 머물면서 조사해도 되냐고 물었잖아요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그리고 저희는 행성을 다치게 하지 않는 선에서 허락했구요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>하지만 나는 요즘 인간들이 무척이나 의심스럽구나</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인간들이 의심스럽다구요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래 최근 무언가 달라진 느낌을 많아 받는구나…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>숲속에 동물들이 많이 보이지 않고 무엇보다 이상한 소음이 늘었어…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>호호야 내가 부탁하나 해도 되겠느냐?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">숲속을 순찰하면서 이상한 것들이 있는지 조사하고 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인간들이 숲속의 변화에 상관이 있는지 알아봐주렴…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내가 괜한 의심을 하는 걸지도 모르지만…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네 그럼요! 족장님의 부탁이신걸요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제가 뭘 도와드리면 될까요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잠시만 호호야</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>혹시 모르니 너에게 몸을 지킬 수 있는 방법을 알려주마</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지킬 수 있는 방법이요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래 WASD를 이용하여 몸을 이동시키고</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Space Bar를 눌러 여우 구슬을 발사하렴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>우리 행성의 부족들이 대대로 부족을 지키는 데 이용한 힘이란다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>으으 아파라…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>숲속에 왜 저런게 있지?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>혹시 모르니 주변을 좀 더 살펴봐야겠어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일단 마을로 돌아가서 족장님께 말씀드려야(쫑긋)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>위이이잉 위이이잉</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>무슨 소리지? 뭐가 위이잉거렸는데?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>흠… 저 소리가 무엇인지만 확인하고 가야겠어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>족장님 의심대로 인간들이 한건가?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">헉헉 내 생각보다 양이 많았어, 저런 위험하고 이상한 물건들이 숲속에 널려있고 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">어떤 물체가 숲속을 막고 있었지 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>여우 구슬로도 부술 수 없고... 다른 물건들과 다르게 아프진 않았지만 수상해</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>확실히 무슨일이 벌어지고 있는 것 확실한것 같네...</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>뭐지? 기존것들과는 다르게 움직였어!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">어떻게 해야하지 으으 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일단 어서 마을로 돌아가ㅇ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일단 조심히 마을로 돌아가ㅇ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>으아 들켰다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>헉헉헉 정말 힘들었어 그리고 저 물체들 점점 더 빨리져서 더 힘들었지…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래도 주변에 있는 것들은 다 처리 한 것 같으니까 이젠 정말 돌아가야겠어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>위이이이이이이이잉!!!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>위우우웅 위이이이이이잉!!!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>삐빅 자원.. 수집 한다… 자우언으…ㅅ우이집…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>말소리?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>누군가 있나?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">말을 이상하게 하긴 하지만 누군가 다친 것 수도 있으니까 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>도와주려 가야겠어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>왜 이렇게 위험한 것들이 많아진거지?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>우리 호호족들만 있었을때는 이런일이 일어나지 않았어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그럼 정말 족장님의 의심대로 인간들이 벌인 짓인가?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 행성 @$^%&amp;$ 수집#%@$%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>또 말소리가 들리잖아</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그러게 원래도 좀 고장이 났어지만 이정도는 아니였는데…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>어쨌든 이 행성의 자원에 대해서는 거의 다 조사했어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래? 결과는?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>우리 지구로 돌아가서도 충분이 사용이 가능한 자원들이야</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지구의 에너지 고갈 사태에 충분한 해결책이 될 것 같아</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래 그럼 이 행성의 원주민들이 알아차리기 전에 최대한 많은 자원을 채굴하자고</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>하! 저 착해빠지고 멍청한 놈들은 우리의 허무맹랑한 소리도 믿었어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>근데 만약 원주민들이 알게 되면 어떻게하지?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래 그럼 곧 철수하지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>방금 무슨 소리 못들었나?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소리? 뭐가?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>흠… 아니다 잘못 들은 모양이군 가지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>말도 안돼… 우리 행성을 자원을 빼앗고 여차하면 공격하겠다니…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>어서 이 사실을 족장님께 말씀드려야지!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주호마을</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인간들이 돌아가고 난 후</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>족장님!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>호호야 돌아왔구나</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이상한 물체들이 날라와 우리를 공격했단다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>하지만 걱정 말거라 여우구슬의 힘으로 부족이 힘을 합쳐 물리쳤으니</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">그래서 숲속에 이상한 것들을 만들었고 무엇보다 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그리고 만약 알게 되더라도 우리가 가지고 있는 장비들을 사용해 모두 처리하면 그만이야</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래 알려줘서 고맙구나 호호야 수고했단다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래… 다른 부족장들과 상의해서 그들을 이 행성에 머물수 있도록 허락했지..</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그리고 위험할 수 있으니 인간을 마주친다면 숨으려무나…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네! 그럼 다녀오겠ㅅ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>여우 구슬이요? 그게 뭐죠?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">이 힘으로 자신과, 부족을 지켜주렴 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네 족장님 인간… 마을이 왜 망가진거죠?!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다행이다… 아 맞다. 족장님 의심이 맞았어요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">인간들은 저의 행성을 연구하는 것이 아닌 자원을 훔치려 온거였어요 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">하긴 그렇긴 하지 그럼 이제 본부로 돌아가자 이 지역에 관한 정보는 거의 다 얻었어 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">이제 다른 지역으로 가도 될 것 같아 이곳을 마지막으로 이 행성의 지역별 자원에 대한 정보는 다 얻었어  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이제 본부로 돌아가서 본격적으로 자원을 채굴하자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로봇103-1177호가 망가졌군</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>호호야 위험하지만 인간들은 본부에 대해 조사를 해봐야겠구나..</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일단 우리가 인간들에 대해 가진 정보가 너무 부족하니…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>만약 최악의 상황이 막치면 이 행성의 모든 부족들을 불러 모아 인간들과 전쟁을 할 수 도 있겠구나…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">일단 마을을 정비하자꾸나 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그리고 준비 해야지 앞으로 우리 부족에게 닥칠 일을…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이번엔 몰래 접근 해야겠어…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">만약 저희가 자기들의 계획을 알게되면 저희를 다 처리할 거라고… </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그리고 본부로 돌아간 다음 다른 지역으로 옮겨 본격적으로 자원을 채굴할 것이라고 했어요</t>
-  </si>
-  <si>
-    <t>네!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Character/00001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주호 족장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>호호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">말까지 하는 이상한 물체.. 정말 위험했어. 대체 숲속에서 무슨일이 일어나고 있는거야 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>???</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>??</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인간1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인간2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>바스락! (헉!)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헉헉 내 생각보다 양이 많았어, 왜 저런 위험하고 이상한 물건들이 숲속에 널려있는 거지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리고 숲속을 막고 있던건 도대체 뭘까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저 ㅈ저건 도대체 뭐지?! 살아있지도 않은데 움직였어!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어떻게 해야하지 으으</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마을로 돌아가야하나? 하지만 아직 인간들에 대한 단서는 못찾았는데…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -880,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -936,16 +949,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>127</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
@@ -968,13 +981,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -1000,13 +1013,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -1032,13 +1045,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -1064,13 +1077,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
@@ -1096,13 +1109,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
@@ -1128,13 +1141,13 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
@@ -1160,13 +1173,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
@@ -1192,13 +1205,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
@@ -1224,13 +1237,13 @@
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
@@ -1256,13 +1269,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
@@ -1288,13 +1301,13 @@
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
@@ -1320,13 +1333,13 @@
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>10</v>
@@ -1352,13 +1365,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>10</v>
@@ -1384,13 +1397,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>10</v>
@@ -1416,13 +1429,13 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>10</v>
@@ -1448,13 +1461,13 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>10</v>
@@ -1480,13 +1493,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>10</v>
@@ -1512,16 +1525,16 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -1544,13 +1557,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>10</v>
@@ -1576,13 +1589,13 @@
         <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>10</v>
@@ -1608,13 +1621,13 @@
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>10</v>
@@ -1640,13 +1653,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>10</v>
@@ -1672,13 +1685,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>10</v>
@@ -1704,13 +1717,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>10</v>
@@ -1736,13 +1749,13 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>10</v>
@@ -1768,13 +1781,13 @@
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>10</v>
@@ -1800,13 +1813,13 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>10</v>
@@ -1832,13 +1845,13 @@
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>10</v>
@@ -1864,13 +1877,13 @@
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>10</v>
@@ -1896,13 +1909,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>10</v>
@@ -1928,13 +1941,13 @@
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>10</v>
@@ -1960,13 +1973,13 @@
         <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>10</v>
@@ -1992,16 +2005,16 @@
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G35" s="1">
         <v>0</v>
@@ -2024,16 +2037,16 @@
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G36" s="1">
         <v>0</v>
@@ -2056,13 +2069,13 @@
         <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>10</v>
@@ -2077,7 +2090,7 @@
         <v>-100</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -2088,16 +2101,16 @@
         <v>0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="G38" s="1">
         <v>0</v>
@@ -2120,16 +2133,16 @@
         <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="G39" s="1">
         <v>0</v>
@@ -2152,16 +2165,16 @@
         <v>0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="G40" s="1">
         <v>0</v>
@@ -2173,7 +2186,7 @@
         <v>-100</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -2184,16 +2197,16 @@
         <v>0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="G41" s="1">
         <v>0</v>
@@ -2216,13 +2229,13 @@
         <v>0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>10</v>
@@ -2248,13 +2261,13 @@
         <v>0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>10</v>
@@ -2280,13 +2293,13 @@
         <v>0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>10</v>
@@ -2312,13 +2325,13 @@
         <v>0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>10</v>
@@ -2344,13 +2357,13 @@
         <v>0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>10</v>
@@ -2376,10 +2389,10 @@
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
@@ -2406,16 +2419,16 @@
         <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G48" s="1">
         <v>0</v>
@@ -2438,16 +2451,16 @@
         <v>0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="G49" s="1">
         <v>0</v>
@@ -2459,7 +2472,7 @@
         <v>-100</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>10</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -2470,16 +2483,16 @@
         <v>0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="G50" s="1">
         <v>0</v>
@@ -2502,13 +2515,13 @@
         <v>0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>61</v>
+        <v>134</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>10</v>
@@ -2534,13 +2547,13 @@
         <v>0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>10</v>
@@ -2566,10 +2579,10 @@
         <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
@@ -2596,16 +2609,16 @@
         <v>0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G54" s="1">
         <v>0</v>
@@ -2628,16 +2641,16 @@
         <v>0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G55" s="1">
         <v>0</v>
@@ -2660,13 +2673,13 @@
         <v>0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>10</v>
@@ -2692,10 +2705,10 @@
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
@@ -2722,13 +2735,13 @@
         <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>10</v>
@@ -2754,13 +2767,13 @@
         <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>10</v>
@@ -2786,16 +2799,16 @@
         <v>0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G60" s="1">
         <v>0</v>
@@ -2818,14 +2831,14 @@
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G61" s="1">
         <v>0</v>
@@ -2848,13 +2861,13 @@
         <v>0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>10</v>
@@ -2880,13 +2893,13 @@
         <v>0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>10</v>
@@ -2912,13 +2925,13 @@
         <v>0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>10</v>
@@ -2944,13 +2957,13 @@
         <v>0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>10</v>
@@ -2976,13 +2989,13 @@
         <v>0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>10</v>
@@ -3008,13 +3021,13 @@
         <v>0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>10</v>
@@ -3040,13 +3053,13 @@
         <v>0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>10</v>
@@ -3072,13 +3085,13 @@
         <v>0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>10</v>
@@ -3104,10 +3117,10 @@
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
@@ -3134,13 +3147,13 @@
         <v>0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>10</v>
@@ -3166,13 +3179,13 @@
         <v>0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>10</v>
@@ -3198,10 +3211,10 @@
         <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
@@ -3228,10 +3241,10 @@
         <v>0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
@@ -3258,10 +3271,10 @@
         <v>0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
@@ -3288,10 +3301,10 @@
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>10</v>
@@ -3317,10 +3330,10 @@
         <v>0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>10</v>
@@ -3346,10 +3359,10 @@
         <v>0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>10</v>
@@ -3375,10 +3388,10 @@
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>10</v>
@@ -3404,10 +3417,10 @@
         <v>0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>10</v>
@@ -3433,10 +3446,10 @@
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>10</v>
@@ -3462,10 +3475,10 @@
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>10</v>
@@ -3491,10 +3504,10 @@
         <v>0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>10</v>
@@ -3520,10 +3533,10 @@
         <v>0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>10</v>
@@ -3549,10 +3562,10 @@
         <v>0</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>10</v>
@@ -3578,10 +3591,10 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>10</v>
@@ -3607,13 +3620,13 @@
         <v>0</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>10</v>
@@ -3639,10 +3652,10 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>10</v>
@@ -3668,10 +3681,10 @@
         <v>0</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>10</v>
@@ -3697,10 +3710,10 @@
         <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>10</v>
@@ -3726,7 +3739,7 @@
         <v>0</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>10</v>
@@ -3752,13 +3765,13 @@
         <v>0</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>10</v>
@@ -3784,13 +3797,13 @@
         <v>0</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>10</v>
@@ -3816,7 +3829,7 @@
         <v>1</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>10</v>
@@ -3842,13 +3855,13 @@
         <v>0</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>10</v>
@@ -3874,13 +3887,13 @@
         <v>1</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>10</v>
@@ -3906,13 +3919,13 @@
         <v>0</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>10</v>
@@ -3938,13 +3951,13 @@
         <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>10</v>
@@ -3970,13 +3983,13 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>10</v>
@@ -4002,13 +4015,13 @@
         <v>0</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>10</v>
@@ -4034,13 +4047,13 @@
         <v>0</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>10</v>
@@ -4066,13 +4079,13 @@
         <v>0</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>10</v>
@@ -4098,13 +4111,13 @@
         <v>0</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>10</v>
@@ -4130,13 +4143,13 @@
         <v>0</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D104" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>10</v>
@@ -4162,13 +4175,13 @@
         <v>1</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>10</v>
@@ -4194,13 +4207,13 @@
         <v>0</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>10</v>
@@ -4226,13 +4239,13 @@
         <v>1</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>10</v>
@@ -4258,13 +4271,13 @@
         <v>1</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>10</v>
@@ -4290,13 +4303,13 @@
         <v>1</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D109" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E109" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>10</v>
@@ -4322,13 +4335,13 @@
         <v>0</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>10</v>
@@ -4354,13 +4367,13 @@
         <v>1</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>10</v>
@@ -4386,13 +4399,13 @@
         <v>1</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>10</v>
@@ -4418,13 +4431,13 @@
         <v>0</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>10</v>
@@ -4447,7 +4460,7 @@
         <v>112</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>10</v>

</xml_diff>